<commit_message>
Fonctionnel pour une liste de liste d'ids et de dates du jour
</commit_message>
<xml_diff>
--- a/Excel/TI/Mon_TI_2024_03_26.xlsx
+++ b/Excel/TI/Mon_TI_2024_03_26.xlsx
@@ -1222,93 +1222,93 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>MIL</t>
+          <t>LAL</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Khris Middleton</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
+          <t>D'Angelo Russell</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Day-To-Day</t>
+        </is>
+      </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>G</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
-        <v>26</v>
+        <v>24.4</v>
       </c>
       <c r="G6" t="n">
-        <v>26.8</v>
+        <v>29.6</v>
       </c>
       <c r="H6" t="n">
-        <v>23.9</v>
+        <v>26.2</v>
       </c>
       <c r="I6" t="n">
+        <v>12</v>
+      </c>
+      <c r="J6" t="n">
+        <v>4</v>
+      </c>
+      <c r="K6" t="n">
         <v>3</v>
       </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" t="n">
-        <v>1</v>
-      </c>
       <c r="L6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M6" t="n">
-        <v>1</v>
-      </c>
-      <c r="N6" t="n">
-        <v>23</v>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O6" t="n">
+        <v>13</v>
       </c>
       <c r="P6" t="n">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="Q6" t="n">
-        <v>36</v>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>35</v>
+      </c>
+      <c r="R6" t="n">
+        <v>7</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="T6" t="n">
-        <v>0.9</v>
+        <v>-1.9</v>
       </c>
       <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
       <c r="W6" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>LAL</t>
+          <t>MIL</t>
         </is>
       </c>
       <c r="Y6" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Z6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="Z6" t="n">
+        <v>74</v>
       </c>
       <c r="AA6" t="inlineStr">
         <is>
@@ -1337,7 +1337,7 @@
       </c>
       <c r="AF6" t="inlineStr">
         <is>
-          <t>NOP</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="AG6" t="inlineStr">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="AH6" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="AI6" t="inlineStr">
@@ -1357,104 +1357,110 @@
       </c>
       <c r="AJ6" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>BKN</t>
         </is>
       </c>
       <c r="AK6" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AL6" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>TOR</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>LAL</t>
+          <t>MIL</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Austin Reaves</t>
+          <t>Khris Middleton</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>F</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
-        <v>28.2</v>
+        <v>26</v>
       </c>
       <c r="G7" t="n">
-        <v>26.4</v>
+        <v>26.8</v>
       </c>
       <c r="H7" t="n">
-        <v>25.6</v>
+        <v>23.9</v>
       </c>
       <c r="I7" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="J7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="L7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N7" t="n">
-        <v>45</v>
-      </c>
-      <c r="O7" t="n">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="P7" t="n">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="Q7" t="n">
-        <v>5</v>
-      </c>
-      <c r="R7" t="n">
-        <v>43</v>
+        <v>36</v>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="T7" t="n">
-        <v>-1.1</v>
+        <v>0.9</v>
       </c>
       <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
       <c r="W7" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="X7" t="inlineStr">
         <is>
-          <t>MIL</t>
+          <t>LAL</t>
         </is>
       </c>
       <c r="Y7" t="inlineStr">
         <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="Z7" t="n">
-        <v>30</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AA7" t="inlineStr">
         <is>
@@ -1483,49 +1489,49 @@
       </c>
       <c r="AF7" t="inlineStr">
         <is>
+          <t>NOP</t>
+        </is>
+      </c>
+      <c r="AG7" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AH7" t="inlineStr">
+        <is>
+          <t>ATL</t>
+        </is>
+      </c>
+      <c r="AI7" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AJ7" t="inlineStr">
+        <is>
+          <t>WAS</t>
+        </is>
+      </c>
+      <c r="AK7" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AL7" t="inlineStr">
+        <is>
           <t>MEM</t>
-        </is>
-      </c>
-      <c r="AG7" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AH7" t="inlineStr">
-        <is>
-          <t>IND</t>
-        </is>
-      </c>
-      <c r="AI7" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AJ7" t="inlineStr">
-        <is>
-          <t>BKN</t>
-        </is>
-      </c>
-      <c r="AK7" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AL7" t="inlineStr">
-        <is>
-          <t>TOR</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>GSW</t>
+          <t>LAL</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Stephen Curry</t>
+          <t>Austin Reaves</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -1536,43 +1542,43 @@
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
-        <v>32.8</v>
+        <v>28.2</v>
       </c>
       <c r="G8" t="n">
-        <v>24.5</v>
+        <v>26.4</v>
       </c>
       <c r="H8" t="n">
-        <v>34</v>
+        <v>25.6</v>
       </c>
       <c r="I8" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K8" t="n">
+        <v>6</v>
+      </c>
+      <c r="L8" t="n">
         <v>3</v>
       </c>
-      <c r="L8" t="n">
+      <c r="M8" t="n">
         <v>2</v>
       </c>
-      <c r="M8" t="n">
-        <v>3</v>
-      </c>
       <c r="N8" t="n">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="O8" t="n">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="P8" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="Q8" t="n">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="R8" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="S8" t="inlineStr">
         <is>
@@ -1580,7 +1586,7 @@
         </is>
       </c>
       <c r="T8" t="n">
-        <v>-0.9</v>
+        <v>-1.1</v>
       </c>
       <c r="U8" t="inlineStr"/>
       <c r="V8" t="inlineStr"/>
@@ -1591,7 +1597,7 @@
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MIL</t>
         </is>
       </c>
       <c r="Y8" t="inlineStr">
@@ -1600,7 +1606,7 @@
         </is>
       </c>
       <c r="Z8" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="AA8" t="inlineStr">
         <is>
@@ -1629,7 +1635,7 @@
       </c>
       <c r="AF8" t="inlineStr">
         <is>
-          <t>ORL</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="AG8" t="inlineStr">
@@ -1639,7 +1645,7 @@
       </c>
       <c r="AH8" t="inlineStr">
         <is>
-          <t>CHA</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="AI8" t="inlineStr">
@@ -1649,17 +1655,17 @@
       </c>
       <c r="AJ8" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>BKN</t>
         </is>
       </c>
       <c r="AK8" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AL8" t="inlineStr">
         <is>
-          <t>DAL</t>
+          <t>TOR</t>
         </is>
       </c>
     </row>
@@ -1671,62 +1677,62 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Andrew Wiggins</t>
+          <t>Stephen Curry</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>G</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
-        <v>20.4</v>
+        <v>32.8</v>
       </c>
       <c r="G9" t="n">
-        <v>20.7</v>
+        <v>24.5</v>
       </c>
       <c r="H9" t="n">
-        <v>17.9</v>
+        <v>34</v>
       </c>
       <c r="I9" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J9" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N9" t="n">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="O9" t="n">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="P9" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>33</v>
+      </c>
+      <c r="R9" t="n">
         <v>42</v>
       </c>
-      <c r="Q9" t="n">
-        <v>9</v>
-      </c>
-      <c r="R9" t="n">
-        <v>19</v>
-      </c>
       <c r="S9" t="inlineStr">
         <is>
           <t>@</t>
         </is>
       </c>
       <c r="T9" t="n">
-        <v>1.2</v>
+        <v>-0.9</v>
       </c>
       <c r="U9" t="inlineStr"/>
       <c r="V9" t="inlineStr"/>
@@ -1746,7 +1752,7 @@
         </is>
       </c>
       <c r="Z9" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="AA9" t="inlineStr">
         <is>
@@ -1812,12 +1818,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>GSW</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Gordon Hayward</t>
+          <t>Andrew Wiggins</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -1828,45 +1834,43 @@
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
-        <v>8.6</v>
+        <v>20.4</v>
       </c>
       <c r="G10" t="n">
-        <v>9</v>
+        <v>20.7</v>
       </c>
       <c r="H10" t="n">
-        <v>17.8</v>
+        <v>17.9</v>
       </c>
       <c r="I10" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="J10" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L10" t="n">
         <v>0</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="N10" t="n">
+        <v>23</v>
       </c>
       <c r="O10" t="n">
         <v>9</v>
       </c>
       <c r="P10" t="n">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="Q10" t="n">
         <v>9</v>
       </c>
       <c r="R10" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="S10" t="inlineStr">
         <is>
@@ -1874,7 +1878,7 @@
         </is>
       </c>
       <c r="T10" t="n">
-        <v>-0.3</v>
+        <v>1.2</v>
       </c>
       <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr"/>
@@ -1885,7 +1889,7 @@
       </c>
       <c r="X10" t="inlineStr">
         <is>
-          <t>NOP</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="Y10" t="inlineStr">
@@ -1894,7 +1898,7 @@
         </is>
       </c>
       <c r="Z10" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AA10" t="inlineStr">
         <is>
@@ -1918,22 +1922,22 @@
       </c>
       <c r="AE10" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AF10" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>ORL</t>
         </is>
       </c>
       <c r="AG10" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AH10" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>CHA</t>
         </is>
       </c>
       <c r="AI10" t="inlineStr">
@@ -1943,65 +1947,61 @@
       </c>
       <c r="AJ10" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>SAS</t>
         </is>
       </c>
       <c r="AK10" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AL10" t="inlineStr">
         <is>
-          <t>PHI</t>
+          <t>DAL</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>LAL</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>D'Angelo Russell</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Out</t>
-        </is>
-      </c>
+          <t>Gordon Hayward</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>F</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
-        <v>24.4</v>
+        <v>8.6</v>
       </c>
       <c r="G11" t="n">
-        <v>29.6</v>
+        <v>9</v>
       </c>
       <c r="H11" t="n">
-        <v>26.2</v>
+        <v>17.8</v>
       </c>
       <c r="I11" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J11" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="K11" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -2009,16 +2009,16 @@
         </is>
       </c>
       <c r="O11" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="P11" t="n">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="Q11" t="n">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="R11" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="S11" t="inlineStr">
         <is>
@@ -2026,7 +2026,7 @@
         </is>
       </c>
       <c r="T11" t="n">
-        <v>-1.9</v>
+        <v>-0.3</v>
       </c>
       <c r="U11" t="inlineStr"/>
       <c r="V11" t="inlineStr"/>
@@ -2037,7 +2037,7 @@
       </c>
       <c r="X11" t="inlineStr">
         <is>
-          <t>MIL</t>
+          <t>NOP</t>
         </is>
       </c>
       <c r="Y11" t="inlineStr">
@@ -2046,7 +2046,7 @@
         </is>
       </c>
       <c r="Z11" t="n">
-        <v>74</v>
+        <v>13</v>
       </c>
       <c r="AA11" t="inlineStr">
         <is>
@@ -2070,22 +2070,22 @@
       </c>
       <c r="AE11" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AF11" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="AG11" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AH11" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="AI11" t="inlineStr">
@@ -2095,7 +2095,7 @@
       </c>
       <c r="AJ11" t="inlineStr">
         <is>
-          <t>BKN</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="AK11" t="inlineStr">
@@ -2105,7 +2105,7 @@
       </c>
       <c r="AL11" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>PHI</t>
         </is>
       </c>
     </row>

</xml_diff>